<commit_message>
Added the region width info to the xlsx file
</commit_message>
<xml_diff>
--- a/src/input/tallyData_70g.xlsx
+++ b/src/input/tallyData_70g.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Left region" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t xml:space="preserve">G</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t xml:space="preserve">…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Region width is 20 cm</t>
   </si>
 </sst>
 </file>
@@ -235,13 +238,13 @@
   </sheetPr>
   <dimension ref="A1:BW72"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -278,6 +281,9 @@
       <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F2" s="3" t="n">
@@ -16384,7 +16390,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -16399,13 +16405,13 @@
   </sheetPr>
   <dimension ref="A1:BW72"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.58"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16442,6 +16448,9 @@
       <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F2" s="3" t="n">
@@ -32548,7 +32557,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>